<commit_message>
delete EUROSTAT from total excel
</commit_message>
<xml_diff>
--- a/mr-dashboards/mr2024/resources/MetadataFailingValidationAllEndpoints.xlsx
+++ b/mr-dashboards/mr2024/resources/MetadataFailingValidationAllEndpoints.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="197">
   <si>
     <t xml:space="preserve">md_failed</t>
   </si>
@@ -480,139 +480,139 @@
     <t xml:space="preserve">917ecef2-030d-4f61-a874-a8fa45dbb1e5</t>
   </si>
   <si>
+    <t xml:space="preserve">FI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3928b8fb-c393-460f-b8d1-fb756fa1cd49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b0259e81-cd1c-4354-bfa2-5cad4c3c7308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e44416c9-082c-4ffe-9b43-e776960f1fa2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b50f8b12-5b04-4648-be93-ee103002e4f3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38126778-f198-4fe3-a71f-81f994ea7401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16a10f8c-5931-49b9-b9b2-923b69d36f15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0f15a1d5-3ae5-4169-8cd0-1e9f14cf8baf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1bae6e77-8e8e-480c-be6b-d9f47f31371b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71c96a8f-fb74-4bc6-9a15-2f798f62a7d4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">470a8afd-bd30-4bc6-a044-cbbc46c89c68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29f5dbeb-474e-42a3-94bc-1b76952299ad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7447eb94-46a8-4995-9fc0-635ff0d2f5c2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9d92d1c4-c4b6-4d8c-8cec-0fc58989615f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04e44bbf-163c-42fa-ab6c-a2114c1eee5b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8e9f6f41-12a5-4c7b-a75e-d0faa7974d4c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cad4f63a-2868-4116-b140-e2b324133207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85a23ec3-62d5-4c15-875d-b6802485b629</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e5584907-90de-424d-8d40-7f7a418e569b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f2e04512-5b00-4fd6-986f-7be30c75eb35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deea5672-2d32-46ae-be07-aec9e4c58849</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7ca98445-49f7-4e1a-9365-627650113b6d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a6d029e3-fbb1-4459-86fd-e74ec0ed1b23</t>
+  </si>
+  <si>
     <t xml:space="preserve">EUROSTAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3928b8fb-c393-460f-b8d1-fb756fa1cd49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b0259e81-cd1c-4354-bfa2-5cad4c3c7308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e44416c9-082c-4ffe-9b43-e776960f1fa2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b50f8b12-5b04-4648-be93-ee103002e4f3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38126778-f198-4fe3-a71f-81f994ea7401</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16a10f8c-5931-49b9-b9b2-923b69d36f15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0f15a1d5-3ae5-4169-8cd0-1e9f14cf8baf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1bae6e77-8e8e-480c-be6b-d9f47f31371b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71c96a8f-fb74-4bc6-9a15-2f798f62a7d4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">470a8afd-bd30-4bc6-a044-cbbc46c89c68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29f5dbeb-474e-42a3-94bc-1b76952299ad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7447eb94-46a8-4995-9fc0-635ff0d2f5c2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9d92d1c4-c4b6-4d8c-8cec-0fc58989615f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04e44bbf-163c-42fa-ab6c-a2114c1eee5b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8e9f6f41-12a5-4c7b-a75e-d0faa7974d4c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cad4f63a-2868-4116-b140-e2b324133207</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85a23ec3-62d5-4c15-875d-b6802485b629</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">e5584907-90de-424d-8d40-7f7a418e569b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f2e04512-5b00-4fd6-986f-7be30c75eb35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deea5672-2d32-46ae-be07-aec9e4c58849</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7ca98445-49f7-4e1a-9365-627650113b6d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a6d029e3-fbb1-4459-86fd-e74ec0ed1b23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
   </si>
 </sst>
 </file>
@@ -858,7 +858,7 @@
       <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.89"/>
@@ -1434,15 +1434,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK1048576"/>
+  <dimension ref="A1:AK37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.57"/>
@@ -5520,9 +5520,6 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
-        <v>196</v>
-      </c>
       <c r="C37" s="0" t="n">
         <f aca="false">SUM(C2:C36)</f>
         <v>29562</v>
@@ -5664,7 +5661,6 @@
         <v>366</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5689,10 +5685,10 @@
       <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="4" style="0" width="6.56"/>
   </cols>
@@ -7281,7 +7277,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>152</v>
+        <v>196</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>153</v>
@@ -7394,7 +7390,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>155</v>
@@ -7507,7 +7503,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>157</v>
@@ -7620,7 +7616,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>159</v>
@@ -7733,7 +7729,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>161</v>
@@ -7846,7 +7842,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>163</v>
@@ -7959,7 +7955,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>165</v>
@@ -8072,7 +8068,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>167</v>
@@ -8185,7 +8181,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>169</v>
@@ -8298,7 +8294,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>171</v>
@@ -8411,7 +8407,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>173</v>
@@ -8524,7 +8520,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>175</v>
@@ -8637,7 +8633,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>177</v>
@@ -8750,7 +8746,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>179</v>
@@ -8863,7 +8859,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>181</v>
@@ -8976,7 +8972,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>183</v>
@@ -9089,7 +9085,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>185</v>
@@ -9202,7 +9198,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>187</v>
@@ -9315,7 +9311,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>189</v>
@@ -9428,7 +9424,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>191</v>
@@ -9541,7 +9537,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>193</v>
@@ -9654,7 +9650,7 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>195</v>
@@ -9767,7 +9763,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">SUM(C2:C36)</f>

</xml_diff>